<commit_message>
arreglo visualizaciones hasta precios de impo de gas
</commit_message>
<xml_diff>
--- a/analisis/resultados/argentina/renta_de_la_tierra_hidrocarburifera_arg.xlsx
+++ b/analisis/resultados/argentina/renta_de_la_tierra_hidrocarburifera_arg.xlsx
@@ -27,6 +27,7 @@
     <sheet name="VBPextTcp" sheetId="18" r:id="rId18"/>
     <sheet name="RTPG_comparacion" sheetId="19" r:id="rId19"/>
     <sheet name="costos_pg_comparacion" sheetId="20" r:id="rId20"/>
+    <sheet name="costos_pg_ccnn" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -659,7 +660,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -745,15 +746,15 @@
         </is>
       </c>
       <c r="C5">
-        <v>0.03105534818247204</v>
+        <v>0.03088050444735144</v>
       </c>
       <c r="D5">
-        <v>0.0151460018386319</v>
+        <v>0.01506072881196834</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -761,15 +762,15 @@
         </is>
       </c>
       <c r="C6">
-        <v>0.03088050444735144</v>
+        <v>0.01705558267174118</v>
       </c>
       <c r="D6">
-        <v>0.01506072881196834</v>
+        <v>0.008652297406568116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -777,15 +778,15 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.01700036049260458</v>
+        <v>0.02481915318002813</v>
       </c>
       <c r="D7">
-        <v>0.008624283194065115</v>
+        <v>0.01319115708972144</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>2002</v>
+        <v>2004</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -793,15 +794,15 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.01705558267174118</v>
+        <v>0.04206247384189609</v>
       </c>
       <c r="D8">
-        <v>0.008652297406568116</v>
+        <v>0.02175024069009673</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>2003</v>
+        <v>2005</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -809,15 +810,15 @@
         </is>
       </c>
       <c r="C9">
-        <v>0.02464732289044106</v>
+        <v>0.07145197800366922</v>
       </c>
       <c r="D9">
-        <v>0.01309983083349207</v>
+        <v>0.03669801646138235</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>2003</v>
+        <v>2006</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -825,15 +826,15 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.02481915318002813</v>
+        <v>0.08373715399541221</v>
       </c>
       <c r="D10">
-        <v>0.01319115708972144</v>
+        <v>0.04259115262203002</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -841,15 +842,15 @@
         </is>
       </c>
       <c r="C11">
-        <v>0.04175519104138921</v>
+        <v>0.08470165314417698</v>
       </c>
       <c r="D11">
-        <v>0.02159134668647552</v>
+        <v>0.04282715090798902</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -857,15 +858,15 @@
         </is>
       </c>
       <c r="C12">
-        <v>0.04206247384189609</v>
+        <v>0.173816994801324</v>
       </c>
       <c r="D12">
-        <v>0.02175024069009673</v>
+        <v>0.08796695621418162</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>2005</v>
+        <v>2009</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -873,15 +874,15 @@
         </is>
       </c>
       <c r="C13">
-        <v>0.07141438879948277</v>
+        <v>0.1090967145916218</v>
       </c>
       <c r="D13">
-        <v>0.03667871049851686</v>
+        <v>0.04771109448102073</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -889,15 +890,15 @@
         </is>
       </c>
       <c r="C14">
-        <v>0.07145197800366922</v>
+        <v>0.1326057658132142</v>
       </c>
       <c r="D14">
-        <v>0.03669801646138235</v>
+        <v>0.06172576809386024</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -905,15 +906,15 @@
         </is>
       </c>
       <c r="C15">
-        <v>0.0834489608996134</v>
+        <v>0.1441267958673157</v>
       </c>
       <c r="D15">
-        <v>0.04244456922932891</v>
+        <v>0.066404450959776</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -921,15 +922,15 @@
         </is>
       </c>
       <c r="C16">
-        <v>0.08373715399541221</v>
+        <v>0.1605540917069948</v>
       </c>
       <c r="D16">
-        <v>0.04259115262203002</v>
+        <v>0.06929965810705864</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -937,15 +938,15 @@
         </is>
       </c>
       <c r="C17">
-        <v>0.08430482041274182</v>
+        <v>0.1193481703324789</v>
       </c>
       <c r="D17">
-        <v>0.04262650293190438</v>
+        <v>0.04968885261331708</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -953,15 +954,15 @@
         </is>
       </c>
       <c r="C18">
-        <v>0.08470165314417698</v>
+        <v>0.1119908204974199</v>
       </c>
       <c r="D18">
-        <v>0.04282715090798902</v>
+        <v>0.04917979648850521</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -969,15 +970,15 @@
         </is>
       </c>
       <c r="C19">
-        <v>0.1733038422409547</v>
+        <v>0.02299706414250339</v>
       </c>
       <c r="D19">
-        <v>0.08770725509082021</v>
+        <v>0.00989292993802224</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -985,15 +986,15 @@
         </is>
       </c>
       <c r="C20">
-        <v>0.173816994801324</v>
+        <v>-0.01535281100395134</v>
       </c>
       <c r="D20">
-        <v>0.08796695621418162</v>
+        <v>-0.006740386188929313</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1001,15 +1002,15 @@
         </is>
       </c>
       <c r="C21">
-        <v>0.1085230881513234</v>
+        <v>0.01926667590122877</v>
       </c>
       <c r="D21">
-        <v>0.04746023133273679</v>
+        <v>0.008387953962747942</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>2009</v>
+        <v>2018</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1017,233 +1018,9 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.1090967145916218</v>
+        <v>0.03764104066734209</v>
       </c>
       <c r="D22">
-        <v>0.04771109448102073</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <v>2010</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C23">
-        <v>0.1324360866808659</v>
-      </c>
-      <c r="D23">
-        <v>0.06164678529315416</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <v>2010</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C24">
-        <v>0.1326057658132142</v>
-      </c>
-      <c r="D24">
-        <v>0.06172576809386024</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <v>2011</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C25">
-        <v>0.1442798864704979</v>
-      </c>
-      <c r="D25">
-        <v>0.06647498536241947</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>2011</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C26">
-        <v>0.1441267958673157</v>
-      </c>
-      <c r="D26">
-        <v>0.066404450959776</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <v>2012</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C27">
-        <v>0.161155273777156</v>
-      </c>
-      <c r="D27">
-        <v>0.06955914518383957</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>2012</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C28">
-        <v>0.1605540917069948</v>
-      </c>
-      <c r="D28">
-        <v>0.06929965810705864</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>2013</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C29">
-        <v>0.1212531728854755</v>
-      </c>
-      <c r="D29">
-        <v>0.05048197236387667</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>2013</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>0.1193481703324789</v>
-      </c>
-      <c r="D30">
-        <v>0.04968885261331708</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>2014</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C31">
-        <v>0.1155107307383424</v>
-      </c>
-      <c r="D31">
-        <v>0.05072553451004562</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>2014</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C32">
-        <v>0.1119908204974199</v>
-      </c>
-      <c r="D32">
-        <v>0.04917979648850521</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>2015</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C33">
-        <v>0.02299706414250339</v>
-      </c>
-      <c r="D33">
-        <v>0.00989292993802224</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>2016</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C34">
-        <v>-0.01535281100395134</v>
-      </c>
-      <c r="D34">
-        <v>-0.006740386188929313</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>2017</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C35">
-        <v>0.01926667590122877</v>
-      </c>
-      <c r="D35">
-        <v>0.008387953962747942</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36">
-        <v>2018</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="C36">
-        <v>0.03764104066734209</v>
-      </c>
-      <c r="D36">
         <v>0.01742539529351357</v>
       </c>
     </row>
@@ -24353,6 +24130,1087 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>anio</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>unidad_produccion</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Q_total</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>unidad_ccnn</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>fuente</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>KTc</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>unidad_costos</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>P_ext</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>KTCGnorm</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Pcost</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pp</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>PvtaPot</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1997</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>530138733.0003897</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F2">
+        <v>5318404090.959862</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H2">
+        <v>18.13395672908327</v>
+      </c>
+      <c r="J2">
+        <v>10.03209869397706</v>
+      </c>
+      <c r="L2">
+        <v>8.101858035106213</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1998</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>544296623.2439395</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F3">
+        <v>3578053079.606754</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H3">
+        <v>11.55911929922439</v>
+      </c>
+      <c r="I3">
+        <v>3626157282.902394</v>
+      </c>
+      <c r="J3">
+        <v>6.573719047312856</v>
+      </c>
+      <c r="K3">
+        <v>6.662097701968005</v>
+      </c>
+      <c r="L3">
+        <v>4.985400251911533</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1999</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>528919287.7598798</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F4">
+        <v>4897064450.533498</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H4">
+        <v>16.2036299936617</v>
+      </c>
+      <c r="I4">
+        <v>4934135775.776606</v>
+      </c>
+      <c r="J4">
+        <v>9.258623317130155</v>
+      </c>
+      <c r="K4">
+        <v>9.32871213049167</v>
+      </c>
+      <c r="L4">
+        <v>6.94500667653154</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>2000</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>547406250.3110944</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F5">
+        <v>7685168494.265782</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H5">
+        <v>27.9307640595735</v>
+      </c>
+      <c r="I5">
+        <v>7762502527.606819</v>
+      </c>
+      <c r="J5">
+        <v>14.03924140416419</v>
+      </c>
+      <c r="K5">
+        <v>14.18051497072849</v>
+      </c>
+      <c r="L5">
+        <v>13.8915226554093</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>2001</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>573618815.8623729</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F6">
+        <v>6413149117.008606</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H6">
+        <v>23.39587260060197</v>
+      </c>
+      <c r="I6">
+        <v>6496493335.795942</v>
+      </c>
+      <c r="J6">
+        <v>11.18015821598729</v>
+      </c>
+      <c r="K6">
+        <v>11.32545369180259</v>
+      </c>
+      <c r="L6">
+        <v>12.21571438461469</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>2002</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>559689726.5490651</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F7">
+        <v>3380454211.647601</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H7">
+        <v>24.9059965634639</v>
+      </c>
+      <c r="I7">
+        <v>3468988823.903041</v>
+      </c>
+      <c r="J7">
+        <v>6.039871827719271</v>
+      </c>
+      <c r="K7">
+        <v>6.198056993634906</v>
+      </c>
+      <c r="L7">
+        <v>18.86612473574463</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>2003</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>580706545.1841915</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F8">
+        <v>4335825124.096769</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H8">
+        <v>30.1449796250912</v>
+      </c>
+      <c r="I8">
+        <v>4441307193.979344</v>
+      </c>
+      <c r="J8">
+        <v>7.466465050297496</v>
+      </c>
+      <c r="K8">
+        <v>7.648109412251635</v>
+      </c>
+      <c r="L8">
+        <v>22.67851457479371</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2004</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>572118575.1295207</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F9">
+        <v>4369193741.807231</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H9">
+        <v>36.16651394674908</v>
+      </c>
+      <c r="I9">
+        <v>4479260149.599262</v>
+      </c>
+      <c r="J9">
+        <v>7.636867481217681</v>
+      </c>
+      <c r="K9">
+        <v>7.82925139003783</v>
+      </c>
+      <c r="L9">
+        <v>28.5296464655314</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>2005</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>555087150.9384625</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F10">
+        <v>4886478506.428919</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H10">
+        <v>48.14787712144361</v>
+      </c>
+      <c r="I10">
+        <v>5024395709.534697</v>
+      </c>
+      <c r="J10">
+        <v>8.803083440442739</v>
+      </c>
+      <c r="K10">
+        <v>9.051543890072329</v>
+      </c>
+      <c r="L10">
+        <v>39.34479368100088</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2006</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>555709123.542582</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F11">
+        <v>6476312653.513421</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H11">
+        <v>58.71126301600694</v>
+      </c>
+      <c r="I11">
+        <v>6635768684.681076</v>
+      </c>
+      <c r="J11">
+        <v>11.65414131088522</v>
+      </c>
+      <c r="K11">
+        <v>11.94108284992482</v>
+      </c>
+      <c r="L11">
+        <v>47.05712170512172</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2007</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>548835951.0330771</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F12">
+        <v>7737077520.580564</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H12">
+        <v>62.8278887947296</v>
+      </c>
+      <c r="I12">
+        <v>7921278708.023595</v>
+      </c>
+      <c r="J12">
+        <v>14.09724983579705</v>
+      </c>
+      <c r="K12">
+        <v>14.43287141287543</v>
+      </c>
+      <c r="L12">
+        <v>48.73063895893256</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>2008</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>542719084.546919</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F13">
+        <v>9156172812.714533</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H13">
+        <v>85.23603883175497</v>
+      </c>
+      <c r="I13">
+        <v>9403497296.417908</v>
+      </c>
+      <c r="J13">
+        <v>16.87092470750025</v>
+      </c>
+      <c r="K13">
+        <v>17.32663833678943</v>
+      </c>
+      <c r="L13">
+        <v>68.36511412425473</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>2009</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>522701913.1994728</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F14">
+        <v>7747287441.269795</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H14">
+        <v>56.2753035685592</v>
+      </c>
+      <c r="I14">
+        <v>7993822896.618885</v>
+      </c>
+      <c r="J14">
+        <v>14.82161676785997</v>
+      </c>
+      <c r="K14">
+        <v>15.29327269473432</v>
+      </c>
+      <c r="L14">
+        <v>41.45368680069923</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2010</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>509518261.3682242</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F15">
+        <v>8981980392.60391</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H15">
+        <v>75.26580553145574</v>
+      </c>
+      <c r="I15">
+        <v>9371260394.272917</v>
+      </c>
+      <c r="J15">
+        <v>17.62837777096416</v>
+      </c>
+      <c r="K15">
+        <v>18.39239357016959</v>
+      </c>
+      <c r="L15">
+        <v>57.63742776049158</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>2011</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>486771900.7096471</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F16">
+        <v>11227701545.3342</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H16">
+        <v>102.7709066424628</v>
+      </c>
+      <c r="I16">
+        <v>11804490305.84093</v>
+      </c>
+      <c r="J16">
+        <v>23.0656320320991</v>
+      </c>
+      <c r="K16">
+        <v>24.25055819498125</v>
+      </c>
+      <c r="L16">
+        <v>79.7052746103637</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2012</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>477050998.3525273</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F17">
+        <v>12587365584.62986</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H17">
+        <v>105.6393477859505</v>
+      </c>
+      <c r="I17">
+        <v>13467961757.65753</v>
+      </c>
+      <c r="J17">
+        <v>26.38578606501133</v>
+      </c>
+      <c r="K17">
+        <v>28.23170227956443</v>
+      </c>
+      <c r="L17">
+        <v>79.25356172093912</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2013</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>458079675.5528591</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F18">
+        <v>13551159354.95851</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H18">
+        <v>95.18008634631269</v>
+      </c>
+      <c r="I18">
+        <v>15033653474.31398</v>
+      </c>
+      <c r="J18">
+        <v>29.58253788187292</v>
+      </c>
+      <c r="K18">
+        <v>32.81886160124825</v>
+      </c>
+      <c r="L18">
+        <v>65.59754846443978</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>2014</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>453687140.0568594</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F19">
+        <v>11613038815.81717</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H19">
+        <v>93.08851800379156</v>
+      </c>
+      <c r="I19">
+        <v>13718663916.48217</v>
+      </c>
+      <c r="J19">
+        <v>25.59702003976075</v>
+      </c>
+      <c r="K19">
+        <v>30.23815908637579</v>
+      </c>
+      <c r="L19">
+        <v>67.49149796403083</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>2015</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>462299665.1479408</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F20">
+        <v>11216779188.96225</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H20">
+        <v>44.50273988574094</v>
+      </c>
+      <c r="I20">
+        <v>14515271399.38203</v>
+      </c>
+      <c r="J20">
+        <v>24.26300522059164</v>
+      </c>
+      <c r="K20">
+        <v>31.39797082642704</v>
+      </c>
+      <c r="L20">
+        <v>20.2397346651493</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>2016</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>452050762.3595363</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F21">
+        <v>9931696410.118053</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H21">
+        <v>38.47750855883071</v>
+      </c>
+      <c r="I21">
+        <v>14877647025.74215</v>
+      </c>
+      <c r="J21">
+        <v>21.97031226820259</v>
+      </c>
+      <c r="K21">
+        <v>32.91145213003599</v>
+      </c>
+      <c r="L21">
+        <v>16.50719629062812</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>2017</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>438212068.9971514</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F22">
+        <v>10124637619.63029</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H22">
+        <v>39.2615822442685</v>
+      </c>
+      <c r="I22">
+        <v>12240230686.66772</v>
+      </c>
+      <c r="J22">
+        <v>23.10442440072572</v>
+      </c>
+      <c r="K22">
+        <v>27.93220806236464</v>
+      </c>
+      <c r="L22">
+        <v>16.15715784354277</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>2018</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BEP</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>455778084.7661767</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>USD tcc</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Empalme CCNN</t>
+        </is>
+      </c>
+      <c r="F23">
+        <v>7994462876.026632</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>USD/boe</t>
+        </is>
+      </c>
+      <c r="H23">
+        <v>65.91465547394193</v>
+      </c>
+      <c r="I23">
+        <v>10185475043.19722</v>
+      </c>
+      <c r="J23">
+        <v>17.54025290647301</v>
+      </c>
+      <c r="K23">
+        <v>22.34744359949331</v>
+      </c>
+      <c r="L23">
+        <v>48.37440256746892</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E84"/>
@@ -91199,7 +92057,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -91369,10 +92227,10 @@
         </is>
       </c>
       <c r="C5">
-        <v>517442505.9149239</v>
+        <v>730301335.8487251</v>
       </c>
       <c r="D5">
-        <v>2536.901620449671</v>
+        <v>1797.478201542031</v>
       </c>
       <c r="E5">
         <v>4386.706834565219</v>
@@ -91384,10 +92242,10 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>59052119.04442418</v>
+        <v>83344218.78733619</v>
       </c>
       <c r="I5">
-        <v>4314707730.757876</v>
+        <v>4290415631.014965</v>
       </c>
       <c r="J5">
         <v>0.03843839330276964</v>
@@ -91395,7 +92253,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -91403,33 +92261,33 @@
         </is>
       </c>
       <c r="C6">
-        <v>730301335.8487251</v>
+        <v>1473222170.820981</v>
       </c>
       <c r="D6">
-        <v>1797.478201542031</v>
+        <v>15392.11274832851</v>
       </c>
       <c r="E6">
-        <v>4386.706834565219</v>
+        <v>9129.705469448012</v>
       </c>
       <c r="F6">
-        <v>4373759849.802301</v>
+        <v>3166401336.164297</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>83344218.78733619</v>
+        <v>277998682.4820834</v>
       </c>
       <c r="I6">
-        <v>4290415631.014965</v>
+        <v>2888402653.682213</v>
       </c>
       <c r="J6">
-        <v>0.03843839330276964</v>
+        <v>0.04838182825389188</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -91437,33 +92295,33 @@
         </is>
       </c>
       <c r="C7">
-        <v>1522782048.211025</v>
+        <v>1578899228.681467</v>
       </c>
       <c r="D7">
-        <v>14891.16698167919</v>
+        <v>19834.21033021627</v>
       </c>
       <c r="E7">
-        <v>9129.705469448012</v>
+        <v>10743.63517886903</v>
       </c>
       <c r="F7">
-        <v>3166401336.164297</v>
+        <v>5643698838.62067</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>287350687.1500068</v>
+        <v>309062464.7559457</v>
       </c>
       <c r="I7">
-        <v>2879050649.01429</v>
+        <v>5334636373.864724</v>
       </c>
       <c r="J7">
-        <v>0.04838182825389188</v>
+        <v>0.05488572451056611</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>2002</v>
+        <v>2004</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -91471,33 +92329,33 @@
         </is>
       </c>
       <c r="C8">
-        <v>1473222170.820981</v>
+        <v>1737002434.853299</v>
       </c>
       <c r="D8">
-        <v>15392.11274832851</v>
+        <v>26039.06690081698</v>
       </c>
       <c r="E8">
-        <v>9129.705469448012</v>
+        <v>10640.13813443311</v>
       </c>
       <c r="F8">
-        <v>3166401336.164297</v>
+        <v>10873866822.51721</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>277998682.4820834</v>
+        <v>322494574.8306521</v>
       </c>
       <c r="I8">
-        <v>2888402653.682213</v>
+        <v>10551372247.68656</v>
       </c>
       <c r="J8">
-        <v>0.04838182825389188</v>
+        <v>0.05730932328517764</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>2003</v>
+        <v>2005</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -91505,33 +92363,33 @@
         </is>
       </c>
       <c r="C9">
-        <v>1767579170.317021</v>
+        <v>2222224426.621827</v>
       </c>
       <c r="D9">
-        <v>17717.01088006587</v>
+        <v>28019.04974059555</v>
       </c>
       <c r="E9">
-        <v>10743.63517886903</v>
+        <v>11419.95224903055</v>
       </c>
       <c r="F9">
-        <v>5643698838.62067</v>
+        <v>21781874496.03072</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>345995719.7430863</v>
+        <v>403879036.1950127</v>
       </c>
       <c r="I9">
-        <v>5297703118.877585</v>
+        <v>21377995459.83571</v>
       </c>
       <c r="J9">
-        <v>0.05488572451056611</v>
+        <v>0.06283489501643001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>2003</v>
+        <v>2006</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -91539,33 +92397,33 @@
         </is>
       </c>
       <c r="C10">
-        <v>1578899228.681467</v>
+        <v>2733519061.788257</v>
       </c>
       <c r="D10">
-        <v>19834.21033021627</v>
+        <v>39604.81290891427</v>
       </c>
       <c r="E10">
-        <v>10743.63517886903</v>
+        <v>12510.53897531976</v>
       </c>
       <c r="F10">
-        <v>5643698838.62067</v>
+        <v>30981953900.10583</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>309062464.7559457</v>
+        <v>490765799.9262488</v>
       </c>
       <c r="I10">
-        <v>5334636373.864724</v>
+        <v>30491188100.17959</v>
       </c>
       <c r="J10">
-        <v>0.05488572451056611</v>
+        <v>0.0696825181531</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -91573,33 +92431,33 @@
         </is>
       </c>
       <c r="C11">
-        <v>2152176675.379988</v>
+        <v>3228392060.754088</v>
       </c>
       <c r="D11">
-        <v>21015.89666194168</v>
+        <v>38295.81044652226</v>
       </c>
       <c r="E11">
-        <v>10640.13813443311</v>
+        <v>14023.74321179328</v>
       </c>
       <c r="F11">
-        <v>10873866822.51721</v>
+        <v>38989659480.28438</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>399576470.3379556</v>
+        <v>574554203.8327217</v>
       </c>
       <c r="I11">
-        <v>10474290352.17926</v>
+        <v>38415105276.45165</v>
       </c>
       <c r="J11">
-        <v>0.05730932328517764</v>
+        <v>0.07879872942360158</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -91607,33 +92465,33 @@
         </is>
       </c>
       <c r="C12">
-        <v>1737002434.853299</v>
+        <v>4439628382.673468</v>
       </c>
       <c r="D12">
-        <v>26039.06690081698</v>
+        <v>44877.08064641061</v>
       </c>
       <c r="E12">
-        <v>10640.13813443311</v>
+        <v>17137.02769645459</v>
       </c>
       <c r="F12">
-        <v>10873866822.51721</v>
+        <v>101918142364.5508</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>322494574.8306521</v>
+        <v>787275052.3751236</v>
       </c>
       <c r="I12">
-        <v>10551372247.68656</v>
+        <v>101130867312.1757</v>
       </c>
       <c r="J12">
-        <v>0.05730932328517764</v>
+        <v>0.09663971229154263</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>2005</v>
+        <v>2009</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -91641,33 +92499,33 @@
         </is>
       </c>
       <c r="C13">
-        <v>2284104733.913166</v>
+        <v>5477529471.915593</v>
       </c>
       <c r="D13">
-        <v>27259.96571865189</v>
+        <v>56777.88587251553</v>
       </c>
       <c r="E13">
-        <v>11419.95224903055</v>
+        <v>18732.93802802496</v>
       </c>
       <c r="F13">
-        <v>21781874496.03072</v>
+        <v>60589372139.76433</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>124792926.892502</v>
       </c>
       <c r="H13">
-        <v>415125496.5294757</v>
+        <v>924507957.5590882</v>
       </c>
       <c r="I13">
-        <v>21366748999.50124</v>
+        <v>59540071255.31274</v>
       </c>
       <c r="J13">
-        <v>0.06283489501643001</v>
+        <v>0.1109890069686252</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -91675,33 +92533,33 @@
         </is>
       </c>
       <c r="C14">
-        <v>2222224426.621827</v>
+        <v>8965268394.051556</v>
       </c>
       <c r="D14">
-        <v>28019.04974059555</v>
+        <v>63882.68683920409</v>
       </c>
       <c r="E14">
-        <v>11419.95224903055</v>
+        <v>23593.09495345317</v>
       </c>
       <c r="F14">
-        <v>21781874496.03072</v>
+        <v>104583815995.8457</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>498516277.7833744</v>
       </c>
       <c r="H14">
-        <v>403879036.1950127</v>
+        <v>1514299206.492437</v>
       </c>
       <c r="I14">
-        <v>21377995459.83571</v>
+        <v>102571000511.57</v>
       </c>
       <c r="J14">
-        <v>0.06283489501643001</v>
+        <v>0.1396807365395046</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -91709,33 +92567,33 @@
         </is>
       </c>
       <c r="C15">
-        <v>3318023131.673309</v>
+        <v>14298018695.65338</v>
       </c>
       <c r="D15">
-        <v>32628.01575782807</v>
+        <v>62634.10166114393</v>
       </c>
       <c r="E15">
-        <v>12510.53897531976</v>
+        <v>28682.76453051643</v>
       </c>
       <c r="F15">
-        <v>30981953900.10583</v>
+        <v>148157013087.2179</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1089512051.815389</v>
       </c>
       <c r="H15">
-        <v>595705476.926206</v>
+        <v>2370601805.682655</v>
       </c>
       <c r="I15">
-        <v>30386248423.17963</v>
+        <v>144696899229.7198</v>
       </c>
       <c r="J15">
-        <v>0.0696825181531</v>
+        <v>0.172996874682735</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -91743,33 +92601,33 @@
         </is>
       </c>
       <c r="C16">
-        <v>2733519061.788257</v>
+        <v>25638194345.43493</v>
       </c>
       <c r="D16">
-        <v>39604.81290891427</v>
+        <v>57238.78185691943</v>
       </c>
       <c r="E16">
-        <v>12510.53897531976</v>
+        <v>33445.93732402004</v>
       </c>
       <c r="F16">
-        <v>30981953900.10583</v>
+        <v>193146451418.3993</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>6330993235.717319</v>
       </c>
       <c r="H16">
-        <v>490765799.9262488</v>
+        <v>4008930385.469017</v>
       </c>
       <c r="I16">
-        <v>30491188100.17959</v>
+        <v>182806527797.213</v>
       </c>
       <c r="J16">
-        <v>0.0696825181531</v>
+        <v>0.2138958172700075</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -91777,33 +92635,33 @@
         </is>
       </c>
       <c r="C17">
-        <v>4239675490.890424</v>
+        <v>53056413806.82304</v>
       </c>
       <c r="D17">
-        <v>29161.16827133157</v>
+        <v>41674.56868438402</v>
       </c>
       <c r="E17">
-        <v>14023.74321179328</v>
+        <v>41311.86946546923</v>
       </c>
       <c r="F17">
-        <v>38989659480.28438</v>
+        <v>184557425155.3833</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>10044925464.68162</v>
       </c>
       <c r="H17">
-        <v>754531460.3483036</v>
+        <v>8138892715.261562</v>
       </c>
       <c r="I17">
-        <v>38235128019.93607</v>
+        <v>166373606975.4402</v>
       </c>
       <c r="J17">
-        <v>0.07879872942360158</v>
+        <v>0.2693068600576771</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -91811,33 +92669,33 @@
         </is>
       </c>
       <c r="C18">
-        <v>3228392060.754088</v>
+        <v>107849076954.4208</v>
       </c>
       <c r="D18">
-        <v>38295.81044652226</v>
+        <v>96959.01730947822</v>
       </c>
       <c r="E18">
-        <v>14023.74321179328</v>
+        <v>60945.45478688894</v>
       </c>
       <c r="F18">
-        <v>38989659480.28438</v>
+        <v>253751510636.2328</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>11447716063.52525</v>
       </c>
       <c r="H18">
-        <v>574554203.8327217</v>
+        <v>17105256067.76217</v>
       </c>
       <c r="I18">
-        <v>38415105276.45165</v>
+        <v>225198538504.9454</v>
       </c>
       <c r="J18">
-        <v>0.07879872942360158</v>
+        <v>0.384262651040995</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -91845,33 +92703,33 @@
         </is>
       </c>
       <c r="C19">
-        <v>6123302845.364932</v>
+        <v>203679532741.7822</v>
       </c>
       <c r="D19">
-        <v>32537.59711070712</v>
+        <v>71335.03507370639</v>
       </c>
       <c r="E19">
-        <v>17137.02769645459</v>
+        <v>74273.23030866738</v>
       </c>
       <c r="F19">
-        <v>101918142364.5508</v>
+        <v>125739406024.687</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>35727065374.15405</v>
       </c>
       <c r="H19">
-        <v>1085839433.56774</v>
+        <v>31104781544.25854</v>
       </c>
       <c r="I19">
-        <v>100832302930.9831</v>
+        <v>58907559106.27439</v>
       </c>
       <c r="J19">
-        <v>0.09663971229154263</v>
+        <v>0.4863540617691473</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -91879,33 +92737,33 @@
         </is>
       </c>
       <c r="C20">
-        <v>4439628382.673468</v>
+        <v>464643895044.9334</v>
       </c>
       <c r="D20">
-        <v>44877.08064641061</v>
+        <v>74812.54260287425</v>
       </c>
       <c r="E20">
-        <v>17137.02769645459</v>
+        <v>106300.4782869667</v>
       </c>
       <c r="F20">
-        <v>101918142364.5508</v>
+        <v>39843576841.67973</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>22216030802.64836</v>
       </c>
       <c r="H20">
-        <v>787275052.3751236</v>
+        <v>73088519074.21626</v>
       </c>
       <c r="I20">
-        <v>101130867312.1757</v>
+        <v>-55460973035.18488</v>
       </c>
       <c r="J20">
-        <v>0.09663971229154263</v>
+        <v>0.6757814893778542</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -91913,33 +92771,33 @@
         </is>
       </c>
       <c r="C21">
-        <v>7332345791.541246</v>
+        <v>222599848984.0219</v>
       </c>
       <c r="D21">
-        <v>42415.14953898425</v>
+        <v>486428.6870707158</v>
       </c>
       <c r="E21">
-        <v>18732.93802802496</v>
+        <v>131183.6492037347</v>
       </c>
       <c r="F21">
-        <v>60589372139.76433</v>
+        <v>145751028095.9135</v>
       </c>
       <c r="G21">
-        <v>124792926.892502</v>
+        <v>21320456989.61691</v>
       </c>
       <c r="H21">
-        <v>1237567422.797288</v>
+        <v>35013065259.46954</v>
       </c>
       <c r="I21">
-        <v>59227011790.07454</v>
+        <v>89417505846.8271</v>
       </c>
       <c r="J21">
-        <v>0.1109890069686252</v>
+        <v>0.834016110429706</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>2009</v>
+        <v>2018</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -91947,503 +92805,27 @@
         </is>
       </c>
       <c r="C22">
-        <v>5477529471.915593</v>
+        <v>542750893000.0001</v>
       </c>
       <c r="D22">
-        <v>56777.88587251553</v>
+        <v>543812.5371795649</v>
       </c>
       <c r="E22">
-        <v>18732.93802802496</v>
+        <v>157437.741</v>
       </c>
       <c r="F22">
-        <v>60589372139.76433</v>
+        <v>367947600890.1384</v>
       </c>
       <c r="G22">
-        <v>124792926.892502</v>
+        <v>29085444296.19057</v>
       </c>
       <c r="H22">
-        <v>924507957.5590882</v>
+        <v>85449474519.65273</v>
       </c>
       <c r="I22">
-        <v>59540071255.31274</v>
+        <v>253412682074.2951</v>
       </c>
       <c r="J22">
-        <v>0.1109890069686252</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <v>2010</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C23">
-        <v>9742306325.149157</v>
-      </c>
-      <c r="D23">
-        <v>58787.45895806568</v>
-      </c>
-      <c r="E23">
-        <v>23593.09495345317</v>
-      </c>
-      <c r="F23">
-        <v>104583815995.8457</v>
-      </c>
-      <c r="G23">
-        <v>498516277.7833744</v>
-      </c>
-      <c r="H23">
-        <v>1645546579.215415</v>
-      </c>
-      <c r="I23">
-        <v>102439753138.847</v>
-      </c>
-      <c r="J23">
-        <v>0.1396807365395046</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <v>2010</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C24">
-        <v>8965268394.051556</v>
-      </c>
-      <c r="D24">
-        <v>63882.68683920409</v>
-      </c>
-      <c r="E24">
-        <v>23593.09495345317</v>
-      </c>
-      <c r="F24">
-        <v>104583815995.8457</v>
-      </c>
-      <c r="G24">
-        <v>498516277.7833744</v>
-      </c>
-      <c r="H24">
-        <v>1514299206.492437</v>
-      </c>
-      <c r="I24">
-        <v>102571000511.57</v>
-      </c>
-      <c r="J24">
-        <v>0.1396807365395046</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <v>2011</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C25">
-        <v>13371017537.61906</v>
-      </c>
-      <c r="D25">
-        <v>66976.47011657103</v>
-      </c>
-      <c r="E25">
-        <v>28682.76453051643</v>
-      </c>
-      <c r="F25">
-        <v>148157013087.2179</v>
-      </c>
-      <c r="G25">
-        <v>1089512051.815389</v>
-      </c>
-      <c r="H25">
-        <v>2216905642.18735</v>
-      </c>
-      <c r="I25">
-        <v>144850595393.2151</v>
-      </c>
-      <c r="J25">
-        <v>0.172996874682735</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>2011</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C26">
-        <v>14298018695.65338</v>
-      </c>
-      <c r="D26">
-        <v>62634.10166114393</v>
-      </c>
-      <c r="E26">
-        <v>28682.76453051643</v>
-      </c>
-      <c r="F26">
-        <v>148157013087.2179</v>
-      </c>
-      <c r="G26">
-        <v>1089512051.815389</v>
-      </c>
-      <c r="H26">
-        <v>2370601805.682655</v>
-      </c>
-      <c r="I26">
-        <v>144696899229.7198</v>
-      </c>
-      <c r="J26">
-        <v>0.172996874682735</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <v>2012</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C27">
-        <v>21260602549.18692</v>
-      </c>
-      <c r="D27">
-        <v>69024.3378544216</v>
-      </c>
-      <c r="E27">
-        <v>33445.93732402004</v>
-      </c>
-      <c r="F27">
-        <v>193146451418.3993</v>
-      </c>
-      <c r="G27">
-        <v>6330993235.717319</v>
-      </c>
-      <c r="H27">
-        <v>3324425832.195617</v>
-      </c>
-      <c r="I27">
-        <v>183491032350.4864</v>
-      </c>
-      <c r="J27">
-        <v>0.2138958172700075</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>2012</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C28">
-        <v>25638194345.43493</v>
-      </c>
-      <c r="D28">
-        <v>57238.78185691943</v>
-      </c>
-      <c r="E28">
-        <v>33445.93732402004</v>
-      </c>
-      <c r="F28">
-        <v>193146451418.3993</v>
-      </c>
-      <c r="G28">
-        <v>6330993235.717319</v>
-      </c>
-      <c r="H28">
-        <v>4008930385.469017</v>
-      </c>
-      <c r="I28">
-        <v>182806527797.213</v>
-      </c>
-      <c r="J28">
-        <v>0.2138958172700075</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>2013</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C29">
-        <v>35744830228.59541</v>
-      </c>
-      <c r="D29">
-        <v>61857.98469874096</v>
-      </c>
-      <c r="E29">
-        <v>41311.86946546923</v>
-      </c>
-      <c r="F29">
-        <v>184557425155.3833</v>
-      </c>
-      <c r="G29">
-        <v>10044925464.68162</v>
-      </c>
-      <c r="H29">
-        <v>5483283122.282263</v>
-      </c>
-      <c r="I29">
-        <v>169029216568.4194</v>
-      </c>
-      <c r="J29">
-        <v>0.2693068600576771</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>2013</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>53056413806.82304</v>
-      </c>
-      <c r="D30">
-        <v>41674.56868438402</v>
-      </c>
-      <c r="E30">
-        <v>41311.86946546923</v>
-      </c>
-      <c r="F30">
-        <v>184557425155.3833</v>
-      </c>
-      <c r="G30">
-        <v>10044925464.68162</v>
-      </c>
-      <c r="H30">
-        <v>8138892715.261562</v>
-      </c>
-      <c r="I30">
-        <v>166373606975.4402</v>
-      </c>
-      <c r="J30">
-        <v>0.2693068600576771</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>2014</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C31">
-        <v>63221677253.48461</v>
-      </c>
-      <c r="D31">
-        <v>165401.1879075634</v>
-      </c>
-      <c r="E31">
-        <v>60945.45478688894</v>
-      </c>
-      <c r="F31">
-        <v>253751510636.2328</v>
-      </c>
-      <c r="G31">
-        <v>11447716063.52525</v>
-      </c>
-      <c r="H31">
-        <v>10027188076.08618</v>
-      </c>
-      <c r="I31">
-        <v>232276606496.6214</v>
-      </c>
-      <c r="J31">
-        <v>0.384262651040995</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>2014</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C32">
-        <v>107849076954.4208</v>
-      </c>
-      <c r="D32">
-        <v>96959.01730947822</v>
-      </c>
-      <c r="E32">
-        <v>60945.45478688894</v>
-      </c>
-      <c r="F32">
-        <v>253751510636.2328</v>
-      </c>
-      <c r="G32">
-        <v>11447716063.52525</v>
-      </c>
-      <c r="H32">
-        <v>17105256067.76217</v>
-      </c>
-      <c r="I32">
-        <v>225198538504.9454</v>
-      </c>
-      <c r="J32">
-        <v>0.384262651040995</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>2015</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C33">
-        <v>203679532741.7822</v>
-      </c>
-      <c r="D33">
-        <v>71335.03507370639</v>
-      </c>
-      <c r="E33">
-        <v>74273.23030866738</v>
-      </c>
-      <c r="F33">
-        <v>125739406024.687</v>
-      </c>
-      <c r="G33">
-        <v>35727065374.15405</v>
-      </c>
-      <c r="H33">
-        <v>31104781544.25854</v>
-      </c>
-      <c r="I33">
-        <v>58907559106.27439</v>
-      </c>
-      <c r="J33">
-        <v>0.4863540617691473</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>2016</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C34">
-        <v>464643895044.9334</v>
-      </c>
-      <c r="D34">
-        <v>74812.54260287425</v>
-      </c>
-      <c r="E34">
-        <v>106300.4782869667</v>
-      </c>
-      <c r="F34">
-        <v>39843576841.67973</v>
-      </c>
-      <c r="G34">
-        <v>22216030802.64836</v>
-      </c>
-      <c r="H34">
-        <v>73088519074.21626</v>
-      </c>
-      <c r="I34">
-        <v>-55460973035.18488</v>
-      </c>
-      <c r="J34">
-        <v>0.6757814893778542</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>2017</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C35">
-        <v>222599848984.0219</v>
-      </c>
-      <c r="D35">
-        <v>486428.6870707158</v>
-      </c>
-      <c r="E35">
-        <v>131183.6492037347</v>
-      </c>
-      <c r="F35">
-        <v>145751028095.9135</v>
-      </c>
-      <c r="G35">
-        <v>21320456989.61691</v>
-      </c>
-      <c r="H35">
-        <v>35013065259.46954</v>
-      </c>
-      <c r="I35">
-        <v>89417505846.8271</v>
-      </c>
-      <c r="J35">
-        <v>0.834016110429706</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36">
-        <v>2018</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Pesos corrientes</t>
-        </is>
-      </c>
-      <c r="C36">
-        <v>542750893000.0001</v>
-      </c>
-      <c r="D36">
-        <v>543812.5371795649</v>
-      </c>
-      <c r="E36">
-        <v>157437.741</v>
-      </c>
-      <c r="F36">
-        <v>367947600890.1384</v>
-      </c>
-      <c r="G36">
-        <v>29085444296.19057</v>
-      </c>
-      <c r="H36">
-        <v>85449474519.65273</v>
-      </c>
-      <c r="I36">
-        <v>253412682074.2951</v>
-      </c>
-      <c r="J36">
         <v>1</v>
       </c>
     </row>

</xml_diff>